<commit_message>
Added the base parameters for the skeleton file
</commit_message>
<xml_diff>
--- a/bin/Database/User_Information/skeleton.xlsx
+++ b/bin/Database/User_Information/skeleton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\User_Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9540B23D-83F3-47DB-9C51-BE53961F76BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9D94D9-140D-448C-8DC9-12D6C2637108}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="3375" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
+    <workbookView xWindow="3555" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Amount" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Place/Person</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,18 +415,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03CE7BD-B2D0-4A23-9F6B-DC8026FC762A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1"/>
-  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,38 +423,142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A2DBD7-70F4-41FB-80F6-FD3DA71A2055}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E302CDA9-0C4B-46A5-8034-BB2274D7D4A0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Redid some of the parameters
</commit_message>
<xml_diff>
--- a/bin/Database/User_Information/skeleton.xlsx
+++ b/bin/Database/User_Information/skeleton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\User_Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9D94D9-140D-448C-8DC9-12D6C2637108}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244B1D8A-DD05-453F-8B59-3EB1347FE1C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
+    <workbookView xWindow="5985" yWindow="4305" windowWidth="21600" windowHeight="11835" activeTab="4" xr2:uid="{1FDF4954-229B-4287-993A-E8DC20E2EDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Amount" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>Amount</t>
   </si>
@@ -46,22 +46,16 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Place</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
-    <t>Place/Person</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Location/Place</t>
+  </si>
+  <si>
+    <t>Location/Place/Person</t>
   </si>
 </sst>
 </file>
@@ -415,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03CE7BD-B2D0-4A23-9F6B-DC8026FC762A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -425,15 +419,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A12A9B-8F6C-4916-BF6E-560EC38CF411}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,16 +433,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -460,15 +446,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DDA284-6D89-4D9A-AAA6-AE14FAD24D46}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,16 +460,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -495,15 +473,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A2DBD7-70F4-41FB-80F6-FD3DA71A2055}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,16 +487,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -530,15 +500,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E302CDA9-0C4B-46A5-8034-BB2274D7D4A0}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,16 +514,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>